<commit_message>
Version 1.3.1; Anpassung Zeiterfassung, Versuch des Anzeigens von Bildern
</commit_message>
<xml_diff>
--- a/Allgemeines/Zeiterfassung.xlsx
+++ b/Allgemeines/Zeiterfassung.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="19">
   <si>
     <t>Madi</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>02.11.17</t>
+  </si>
+  <si>
+    <t>03.11.17</t>
   </si>
 </sst>
 </file>
@@ -473,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -920,6 +923,78 @@
       </c>
       <c r="D47" s="7"/>
     </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+    </row>
+    <row r="51" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A51" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+    </row>
+    <row r="52" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A52" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+    </row>
+    <row r="53" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A53" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" s="6"/>
+    </row>
+    <row r="54" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+    </row>
+    <row r="55" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A55" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7">
+        <v>1</v>
+      </c>
+      <c r="D55" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Version 1.4; Passwort ändern
</commit_message>
<xml_diff>
--- a/Allgemeines/Zeiterfassung.xlsx
+++ b/Allgemeines/Zeiterfassung.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="20">
   <si>
     <t>Madi</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>03.11.17</t>
+  </si>
+  <si>
+    <t>04.11.17</t>
   </si>
 </sst>
 </file>
@@ -476,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -995,6 +998,76 @@
       </c>
       <c r="D55" s="7"/>
     </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A57" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A58" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+    </row>
+    <row r="59" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A59" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+    </row>
+    <row r="60" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+    </row>
+    <row r="61" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A61" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" s="6"/>
+    </row>
+    <row r="62" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A62" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+    </row>
+    <row r="63" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A63" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Version 1.5.1; Zweite Datenbank&Zeiterfassung
</commit_message>
<xml_diff>
--- a/Allgemeines/Zeiterfassung.xlsx
+++ b/Allgemeines/Zeiterfassung.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="24">
   <si>
     <t>Madi</t>
   </si>
@@ -93,13 +93,19 @@
   </si>
   <si>
     <t>0.5</t>
+  </si>
+  <si>
+    <t>06.11.17</t>
+  </si>
+  <si>
+    <t>07.11.17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -135,8 +141,15 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,6 +160,12 @@
       <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -168,7 +187,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -182,8 +201,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -196,20 +219,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="17">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -485,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1144,6 +1172,158 @@
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
     </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="8"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+    </row>
+    <row r="73" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A73" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A74" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+    </row>
+    <row r="75" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A75" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+    </row>
+    <row r="76" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A76" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+    </row>
+    <row r="77" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A77" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D77" s="6"/>
+    </row>
+    <row r="78" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A78" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A79" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" s="7">
+        <v>1</v>
+      </c>
+      <c r="C79" s="7">
+        <v>1</v>
+      </c>
+      <c r="D79" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="8"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+    </row>
+    <row r="81" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A81" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A82" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+    </row>
+    <row r="83" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A83" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+    </row>
+    <row r="84" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A84" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+    </row>
+    <row r="85" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A85" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D85" s="6"/>
+    </row>
+    <row r="86" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A86" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+    </row>
+    <row r="87" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A87" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" s="7"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>